<commit_message>
some commit with new computer
</commit_message>
<xml_diff>
--- a/data/single-cell/zeisel_2018/Taxonomy_Symbol-to-Group_Name.xlsx
+++ b/data/single-cell/zeisel_2018/Taxonomy_Symbol-to-Group_Name.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/linhe_xu_vanderbilt_edu/Documents/Herculano_Lab/Projects/neuron-glia-dNdS/data/single-cell/zeisel_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{4A0DCF11-8415-C84B-B574-7EE3C36DC122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FC129E3-479C-D642-B398-50562A4FF9EB}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{4A0DCF11-8415-C84B-B574-7EE3C36DC122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7799599-899F-E34F-8BC8-962B8597C764}"/>
   <bookViews>
-    <workbookView xWindow="34320" yWindow="-6920" windowWidth="26840" windowHeight="14560" xr2:uid="{90CA2813-2ACB-BA49-8F5D-1F7C873FAB07}"/>
+    <workbookView xWindow="34560" yWindow="-8360" windowWidth="26840" windowHeight="14560" xr2:uid="{90CA2813-2ACB-BA49-8F5D-1F7C873FAB07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
   <si>
     <t>Cbnn</t>
   </si>
@@ -282,6 +282,24 @@
   </si>
   <si>
     <t>Spinal cord excitatory neurons</t>
+  </si>
+  <si>
+    <t>inh_neuron</t>
+  </si>
+  <si>
+    <t>exc_neuron</t>
+  </si>
+  <si>
+    <t>excitable</t>
+  </si>
+  <si>
+    <t>endothelia</t>
+  </si>
+  <si>
+    <t>meninges</t>
+  </si>
+  <si>
+    <t>immune</t>
   </si>
 </sst>
 </file>
@@ -648,9 +666,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C11A56D-0670-AD4A-8822-7F5B57EF0E6B}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -658,7 +678,7 @@
     <col min="2" max="2" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -666,15 +686,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -682,7 +705,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -690,23 +713,29 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -714,7 +743,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -722,7 +751,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -730,7 +759,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -738,7 +767,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -746,7 +775,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -754,7 +783,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -762,7 +791,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -770,7 +799,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -778,7 +807,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -786,7 +815,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -794,7 +823,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -802,7 +831,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -810,7 +839,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -818,7 +847,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -826,7 +855,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -834,23 +863,29 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -858,15 +893,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -874,7 +912,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -882,7 +920,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -890,84 +928,114 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>72</v>
+      </c>
+      <c r="C39" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>